<commit_message>
Added contribution for Assignment 2.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49015A7F-194F-3049-9C8B-82FD6B563BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC07986-3F7E-7C4B-B2E3-71970776A5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41140" yWindow="1180" windowWidth="38400" windowHeight="19460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="1180" windowWidth="38400" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Height</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>identified gender (male/female/other)</t>
-  </si>
-  <si>
-    <t>Hair Color</t>
   </si>
   <si>
     <t>BMI</t>
@@ -433,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -450,10 +447,10 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -467,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>0.2</v>
@@ -484,7 +481,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>0.2</v>
@@ -501,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>0.2</v>
@@ -518,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>0.1</v>
@@ -535,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>0.08</v>
@@ -552,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>0.09</v>
@@ -569,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>0.2</v>
@@ -586,7 +583,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>0.2</v>
@@ -603,7 +600,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>0.2</v>
@@ -620,7 +617,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>0.1</v>
@@ -634,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>0.08</v>
@@ -651,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>0.09</v>
@@ -668,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <v>0.23</v>
@@ -685,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>0.55000000000000004</v>
@@ -700,7 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -757,24 +754,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>